<commit_message>
added show_recommandation_by_attendance() and show_table()
</commit_message>
<xml_diff>
--- a/data/movie_data.xlsx
+++ b/data/movie_data.xlsx
@@ -1,13 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\YW\mini_project\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="630" yWindow="525" windowWidth="20175" windowHeight="10125"/>
   </bookViews>
   <sheets>
-    <sheet name="new_name" sheetId="1" r:id="rId1"/>
+    <sheet name="movie_data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -1340,7 +1345,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1413,6 +1418,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1705,17 +1713,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
-      <selection activeCell="B190" sqref="B190"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.375" customWidth="1"/>
     <col min="2" max="2" width="17.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1744,7 +1752,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1773,7 +1781,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1802,7 +1810,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -1831,7 +1839,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -1860,7 +1868,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -1889,7 +1897,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1918,7 +1926,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -1947,7 +1955,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -1976,7 +1984,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -2005,7 +2013,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -2034,7 +2042,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -2063,7 +2071,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>50</v>
       </c>
@@ -2092,7 +2100,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>51</v>
       </c>
@@ -2121,7 +2129,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>54</v>
       </c>
@@ -2150,7 +2158,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>55</v>
       </c>
@@ -2179,7 +2187,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>57</v>
       </c>
@@ -2208,7 +2216,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>60</v>
       </c>
@@ -2237,7 +2245,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>62</v>
       </c>
@@ -2266,7 +2274,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>64</v>
       </c>
@@ -2295,7 +2303,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>66</v>
       </c>
@@ -2324,7 +2332,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>71</v>
       </c>
@@ -2353,7 +2361,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>73</v>
       </c>
@@ -2382,7 +2390,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>75</v>
       </c>
@@ -2411,7 +2419,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>78</v>
       </c>
@@ -2440,7 +2448,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>79</v>
       </c>
@@ -2469,7 +2477,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>81</v>
       </c>
@@ -2498,7 +2506,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>83</v>
       </c>
@@ -2527,7 +2535,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>86</v>
       </c>
@@ -2556,7 +2564,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>89</v>
       </c>
@@ -2585,7 +2593,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>92</v>
       </c>
@@ -2614,7 +2622,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>94</v>
       </c>
@@ -2643,7 +2651,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>97</v>
       </c>
@@ -2672,7 +2680,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>99</v>
       </c>
@@ -2701,7 +2709,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>101</v>
       </c>
@@ -2730,7 +2738,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>103</v>
       </c>
@@ -2759,7 +2767,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>106</v>
       </c>
@@ -2788,7 +2796,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>108</v>
       </c>
@@ -2817,7 +2825,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>110</v>
       </c>
@@ -2846,7 +2854,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>113</v>
       </c>
@@ -2875,7 +2883,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>116</v>
       </c>
@@ -2904,7 +2912,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>119</v>
       </c>
@@ -2933,7 +2941,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>122</v>
       </c>
@@ -2962,7 +2970,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>123</v>
       </c>
@@ -2991,7 +2999,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>125</v>
       </c>
@@ -3020,7 +3028,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>128</v>
       </c>
@@ -3049,7 +3057,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>129</v>
       </c>
@@ -3078,7 +3086,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>130</v>
       </c>
@@ -3107,7 +3115,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>131</v>
       </c>
@@ -3136,7 +3144,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>133</v>
       </c>
@@ -3165,7 +3173,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>134</v>
       </c>
@@ -3194,7 +3202,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>136</v>
       </c>
@@ -3223,7 +3231,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>138</v>
       </c>
@@ -3252,7 +3260,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>140</v>
       </c>
@@ -3281,7 +3289,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>142</v>
       </c>
@@ -3310,7 +3318,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>143</v>
       </c>
@@ -3339,7 +3347,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>145</v>
       </c>
@@ -3368,7 +3376,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>148</v>
       </c>
@@ -3397,7 +3405,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>150</v>
       </c>
@@ -3426,7 +3434,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>153</v>
       </c>
@@ -3455,7 +3463,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>156</v>
       </c>
@@ -3484,7 +3492,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>159</v>
       </c>
@@ -3513,7 +3521,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>161</v>
       </c>
@@ -3542,7 +3550,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>164</v>
       </c>
@@ -3571,7 +3579,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>165</v>
       </c>
@@ -3600,7 +3608,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="66" spans="1:9">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>167</v>
       </c>
@@ -3629,7 +3637,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>169</v>
       </c>
@@ -3658,7 +3666,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>171</v>
       </c>
@@ -3687,7 +3695,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>173</v>
       </c>
@@ -3716,7 +3724,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>176</v>
       </c>
@@ -3745,7 +3753,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>178</v>
       </c>
@@ -3774,7 +3782,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>180</v>
       </c>
@@ -3803,7 +3811,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="73" spans="1:9">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>182</v>
       </c>
@@ -3832,7 +3840,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="74" spans="1:9">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>184</v>
       </c>
@@ -3861,7 +3869,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="75" spans="1:9">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>186</v>
       </c>
@@ -3890,7 +3898,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="76" spans="1:9">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>188</v>
       </c>
@@ -3919,7 +3927,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="77" spans="1:9">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>190</v>
       </c>
@@ -3948,7 +3956,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="78" spans="1:9">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>192</v>
       </c>
@@ -3977,7 +3985,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="79" spans="1:9">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>193</v>
       </c>
@@ -4006,7 +4014,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="80" spans="1:9">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>195</v>
       </c>
@@ -4035,7 +4043,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="81" spans="1:9">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>197</v>
       </c>
@@ -4064,7 +4072,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="82" spans="1:9">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>201</v>
       </c>
@@ -4093,7 +4101,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="83" spans="1:9">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>203</v>
       </c>
@@ -4122,7 +4130,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="84" spans="1:9">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>206</v>
       </c>
@@ -4151,7 +4159,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="85" spans="1:9">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>208</v>
       </c>
@@ -4180,7 +4188,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="86" spans="1:9">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>210</v>
       </c>
@@ -4209,7 +4217,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="87" spans="1:9">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>212</v>
       </c>
@@ -4238,7 +4246,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="88" spans="1:9">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>215</v>
       </c>
@@ -4267,7 +4275,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="89" spans="1:9">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>218</v>
       </c>
@@ -4296,7 +4304,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="90" spans="1:9">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>220</v>
       </c>
@@ -4325,7 +4333,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="91" spans="1:9">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>222</v>
       </c>
@@ -4354,7 +4362,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="92" spans="1:9">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>225</v>
       </c>
@@ -4383,7 +4391,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="93" spans="1:9">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>227</v>
       </c>
@@ -4412,7 +4420,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="94" spans="1:9">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>228</v>
       </c>
@@ -4441,7 +4449,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="95" spans="1:9">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>230</v>
       </c>
@@ -4470,7 +4478,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="96" spans="1:9">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>232</v>
       </c>
@@ -4499,7 +4507,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="97" spans="1:9">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>234</v>
       </c>
@@ -4528,7 +4536,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="98" spans="1:9">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>237</v>
       </c>
@@ -4557,7 +4565,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="99" spans="1:9">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>240</v>
       </c>
@@ -4586,7 +4594,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="100" spans="1:9">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>242</v>
       </c>
@@ -4615,7 +4623,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="101" spans="1:9">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>245</v>
       </c>
@@ -4644,7 +4652,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="102" spans="1:9">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>247</v>
       </c>
@@ -4673,7 +4681,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="103" spans="1:9">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>250</v>
       </c>
@@ -4702,7 +4710,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="104" spans="1:9">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>252</v>
       </c>
@@ -4731,7 +4739,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="105" spans="1:9">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>254</v>
       </c>
@@ -4760,7 +4768,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="106" spans="1:9">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>257</v>
       </c>
@@ -4789,7 +4797,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="107" spans="1:9">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>259</v>
       </c>
@@ -4818,7 +4826,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="108" spans="1:9">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>262</v>
       </c>
@@ -4847,7 +4855,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="109" spans="1:9">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>264</v>
       </c>
@@ -4876,7 +4884,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="110" spans="1:9">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>267</v>
       </c>
@@ -4905,7 +4913,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="111" spans="1:9">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>269</v>
       </c>
@@ -4934,7 +4942,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="112" spans="1:9">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>271</v>
       </c>
@@ -4963,7 +4971,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="113" spans="1:9">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>273</v>
       </c>
@@ -4992,7 +5000,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="114" spans="1:9">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>275</v>
       </c>
@@ -5021,7 +5029,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="115" spans="1:9">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>278</v>
       </c>
@@ -5050,7 +5058,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="116" spans="1:9">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>280</v>
       </c>
@@ -5079,7 +5087,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="117" spans="1:9">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>281</v>
       </c>
@@ -5108,7 +5116,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="118" spans="1:9">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>282</v>
       </c>
@@ -5137,7 +5145,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="119" spans="1:9">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>286</v>
       </c>
@@ -5166,7 +5174,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="120" spans="1:9">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>287</v>
       </c>
@@ -5195,7 +5203,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="121" spans="1:9">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>289</v>
       </c>
@@ -5224,7 +5232,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="122" spans="1:9">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>292</v>
       </c>
@@ -5253,7 +5261,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="123" spans="1:9">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>294</v>
       </c>
@@ -5282,7 +5290,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="124" spans="1:9">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>296</v>
       </c>
@@ -5311,7 +5319,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="125" spans="1:9">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>297</v>
       </c>
@@ -5340,7 +5348,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="126" spans="1:9">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>300</v>
       </c>
@@ -5369,7 +5377,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="127" spans="1:9">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>303</v>
       </c>
@@ -5398,7 +5406,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="128" spans="1:9">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>306</v>
       </c>
@@ -5427,7 +5435,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="129" spans="1:9">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>309</v>
       </c>
@@ -5456,7 +5464,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="130" spans="1:9">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>311</v>
       </c>
@@ -5485,7 +5493,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="131" spans="1:9">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>313</v>
       </c>
@@ -5514,7 +5522,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="132" spans="1:9">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>314</v>
       </c>
@@ -5543,7 +5551,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="133" spans="1:9">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>316</v>
       </c>
@@ -5572,7 +5580,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="134" spans="1:9">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>317</v>
       </c>
@@ -5601,7 +5609,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="135" spans="1:9">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>318</v>
       </c>
@@ -5630,7 +5638,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="136" spans="1:9">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>320</v>
       </c>
@@ -5659,7 +5667,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="137" spans="1:9">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>322</v>
       </c>
@@ -5688,7 +5696,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="138" spans="1:9">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>324</v>
       </c>
@@ -5717,7 +5725,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="139" spans="1:9">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>326</v>
       </c>
@@ -5746,7 +5754,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="140" spans="1:9">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>328</v>
       </c>
@@ -5775,7 +5783,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="141" spans="1:9">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>330</v>
       </c>
@@ -5804,7 +5812,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="142" spans="1:9">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>333</v>
       </c>
@@ -5833,7 +5841,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="143" spans="1:9">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>335</v>
       </c>
@@ -5862,7 +5870,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="144" spans="1:9">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>337</v>
       </c>
@@ -5891,7 +5899,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="145" spans="1:9">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>338</v>
       </c>
@@ -5920,7 +5928,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="146" spans="1:9">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>339</v>
       </c>
@@ -5949,7 +5957,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="147" spans="1:9">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>342</v>
       </c>
@@ -5978,7 +5986,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="148" spans="1:9">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>343</v>
       </c>
@@ -6007,7 +6015,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="149" spans="1:9">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>346</v>
       </c>
@@ -6036,7 +6044,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="150" spans="1:9">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>348</v>
       </c>
@@ -6065,7 +6073,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="151" spans="1:9">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>351</v>
       </c>
@@ -6094,7 +6102,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="152" spans="1:9">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>352</v>
       </c>
@@ -6123,7 +6131,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="153" spans="1:9">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>355</v>
       </c>
@@ -6152,7 +6160,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="154" spans="1:9">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>357</v>
       </c>
@@ -6181,7 +6189,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="155" spans="1:9">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>359</v>
       </c>
@@ -6210,7 +6218,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="156" spans="1:9">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>362</v>
       </c>
@@ -6239,7 +6247,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="157" spans="1:9">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>364</v>
       </c>
@@ -6268,7 +6276,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="158" spans="1:9">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>366</v>
       </c>
@@ -6297,7 +6305,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="159" spans="1:9">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>368</v>
       </c>
@@ -6326,7 +6334,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="160" spans="1:9">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>369</v>
       </c>
@@ -6355,7 +6363,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="161" spans="1:9">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>370</v>
       </c>
@@ -6384,7 +6392,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="162" spans="1:9">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>371</v>
       </c>
@@ -6413,7 +6421,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="163" spans="1:9">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>373</v>
       </c>
@@ -6442,7 +6450,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="164" spans="1:9">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>375</v>
       </c>
@@ -6471,7 +6479,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="165" spans="1:9">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>377</v>
       </c>
@@ -6500,7 +6508,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="166" spans="1:9">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>379</v>
       </c>
@@ -6529,7 +6537,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="167" spans="1:9">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>382</v>
       </c>
@@ -6558,7 +6566,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="168" spans="1:9">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>385</v>
       </c>
@@ -6587,7 +6595,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="169" spans="1:9">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>388</v>
       </c>
@@ -6616,7 +6624,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="170" spans="1:9">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>390</v>
       </c>
@@ -6645,7 +6653,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="171" spans="1:9">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>392</v>
       </c>
@@ -6674,7 +6682,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="172" spans="1:9">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>395</v>
       </c>
@@ -6703,7 +6711,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="173" spans="1:9">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>396</v>
       </c>
@@ -6732,7 +6740,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="174" spans="1:9">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>398</v>
       </c>
@@ -6761,7 +6769,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="175" spans="1:9">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>401</v>
       </c>
@@ -6790,7 +6798,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="176" spans="1:9">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>403</v>
       </c>
@@ -6819,7 +6827,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="177" spans="1:9">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>405</v>
       </c>
@@ -6848,7 +6856,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="178" spans="1:9">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>407</v>
       </c>
@@ -6877,7 +6885,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="179" spans="1:9">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>410</v>
       </c>
@@ -6906,7 +6914,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="180" spans="1:9">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>413</v>
       </c>
@@ -6935,7 +6943,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="181" spans="1:9">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>415</v>
       </c>
@@ -6964,7 +6972,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="182" spans="1:9">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>417</v>
       </c>
@@ -6993,7 +7001,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="183" spans="1:9">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>419</v>
       </c>
@@ -7022,7 +7030,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="184" spans="1:9">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>422</v>
       </c>
@@ -7051,7 +7059,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="185" spans="1:9">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>424</v>
       </c>
@@ -7080,7 +7088,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="186" spans="1:9">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>426</v>
       </c>
@@ -7109,7 +7117,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="187" spans="1:9">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>429</v>
       </c>
@@ -7138,7 +7146,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="188" spans="1:9">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>431</v>
       </c>
@@ -7167,7 +7175,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="189" spans="1:9">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>434</v>
       </c>
@@ -7196,7 +7204,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="190" spans="1:9">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>436</v>
       </c>
@@ -7225,7 +7233,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="191" spans="1:9">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>437</v>
       </c>
@@ -7254,7 +7262,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="192" spans="1:9">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>438</v>
       </c>

</xml_diff>